<commit_message>
Add: File contains user details along with order history & checkOut / checkIn information
</commit_message>
<xml_diff>
--- a/reports/reportPrint.xlsx
+++ b/reports/reportPrint.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -388,7 +388,22 @@
         <v>UserID</v>
       </c>
       <c r="C1" t="str">
+        <v>CheckInDate</v>
+      </c>
+      <c r="D1" t="str">
+        <v>CheckOutDate</v>
+      </c>
+      <c r="E1" t="str">
+        <v>StayDuration</v>
+      </c>
+      <c r="F1" t="str">
+        <v>ChargesOfStay</v>
+      </c>
+      <c r="G1" t="str">
         <v>OrdersOfUser</v>
+      </c>
+      <c r="H1" t="str">
+        <v>TotalBill</v>
       </c>
     </row>
     <row r="2">
@@ -396,10 +411,25 @@
         <v>Abhishek Shigavan</v>
       </c>
       <c r="B2" t="str">
-        <v>Abhi1234</v>
+        <v>Abhi9876</v>
       </c>
       <c r="C2" t="str">
-        <v xml:space="preserve">1. Name Of Item : Breakfast, Quantity : 2, Price : 150, TotalAmount : 354 | 2. Name Of Item : Blanket, Quantity : 2, Price : 400, TotalAmount : 944 | </v>
+        <v>10/04/2021</v>
+      </c>
+      <c r="D2" t="str">
+        <v>10/04/2021</v>
+      </c>
+      <c r="E2" t="str">
+        <v>0 Day 0 Hours</v>
+      </c>
+      <c r="F2">
+        <v>590</v>
+      </c>
+      <c r="G2" t="str">
+        <v xml:space="preserve">1. Name Of Item : Breakfast, Quantity : 2, Price : 150, TotalAmount : 354 | 2. Name Of Item : Bedsheet, Quantity : 2, Price : 300, TotalAmount : 708 | 3. Name Of Item : Dinner, Quantity : 2, Price : 300, TotalAmount : 708 | </v>
+      </c>
+      <c r="H2">
+        <v>2360</v>
       </c>
     </row>
     <row r="3">
@@ -407,15 +437,56 @@
         <v>Peter Parkar</v>
       </c>
       <c r="B3" t="str">
-        <v>Pete1234</v>
+        <v>Pete9988</v>
       </c>
       <c r="C3" t="str">
-        <v xml:space="preserve">1. Name Of Item : Dinner, Quantity : 4, Price : 300, TotalAmount : 1416 | 2. Name Of Item : Tea, Quantity : 4, Price : 25, TotalAmount : 118 | 3. Name Of Item : Pillow, Quantity : 2, Price : 150, TotalAmount : 354 | </v>
+        <v>10/04/2021</v>
+      </c>
+      <c r="D3" t="str">
+        <v>10/04/2021</v>
+      </c>
+      <c r="E3" t="str">
+        <v>0 Day 0 Hours</v>
+      </c>
+      <c r="F3">
+        <v>590</v>
+      </c>
+      <c r="G3" t="str">
+        <v xml:space="preserve">1. Name Of Item : Tea, Quantity : 4, Price : 25, TotalAmount : 118 | 2. Name Of Item : Soap, Quantity : 1, Price : 40, TotalAmount : 47.2 | </v>
+      </c>
+      <c r="H3">
+        <v>755.2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Rajat Sawarkar</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Raja9899</v>
+      </c>
+      <c r="C4" t="str">
+        <v>10/04/2021</v>
+      </c>
+      <c r="D4" t="str">
+        <v>10/04/2021</v>
+      </c>
+      <c r="E4" t="str">
+        <v>0 Day 0 Hours</v>
+      </c>
+      <c r="F4">
+        <v>590</v>
+      </c>
+      <c r="G4" t="str">
+        <v xml:space="preserve">1. Name Of Item : Breakfast, Quantity : 3, Price : 150, TotalAmount : 531 | 2. Name Of Item : Blanket, Quantity : 2, Price : 400, TotalAmount : 944 | </v>
+      </c>
+      <c r="H4">
+        <v>2065</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>